<commit_message>
Scripts renumerados 01-05, tablas con N y modelos (R2/RMSE), train_ml con modelo único y seed
Made-with: Cursor
</commit_message>
<xml_diff>
--- a/data/processed/tabla_resultados_ml_tesina.xlsx
+++ b/data/processed/tabla_resultados_ml_tesina.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,7 @@
     <col width="14" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -456,25 +457,30 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
+          <t>N</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
           <t>Promedio</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>Desv. Est.</t>
         </is>
       </c>
-      <c r="D3" s="2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Mín</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>Máx.</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>Diferencia de medias</t>
         </is>
@@ -511,6 +517,11 @@
           <t>(6)</t>
         </is>
       </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>(7)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -518,27 +529,30 @@
           <t>Datos originales</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="3" t="n">
+        <v>1236</v>
+      </c>
+      <c r="C5" s="3" t="inlineStr">
         <is>
           <t>0.0001</t>
         </is>
       </c>
-      <c r="C5" s="3" t="inlineStr">
+      <c r="D5" s="3" t="inlineStr">
         <is>
           <t>1.0164</t>
         </is>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="E5" s="3" t="inlineStr">
         <is>
           <t>-5.1993</t>
         </is>
       </c>
-      <c r="E5" s="3" t="inlineStr">
+      <c r="F5" s="3" t="inlineStr">
         <is>
           <t>5.1993</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="G5" s="3" t="inlineStr">
         <is>
           <t>—</t>
         </is>
@@ -550,29 +564,32 @@
           <t>KNN</t>
         </is>
       </c>
-      <c r="B6" s="3" t="inlineStr">
-        <is>
-          <t>0.0454</t>
-        </is>
+      <c r="B6" s="3" t="n">
+        <v>5000</v>
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>0.6659</t>
+          <t>0.0382</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
-          <t>-1.7800</t>
+          <t>0.6675</t>
         </is>
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t>2.1804</t>
+          <t>-1.7669</t>
         </is>
       </c>
       <c r="F6" s="3" t="inlineStr">
         <is>
-          <t>0.0453</t>
+          <t>2.5278</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>0.0381</t>
         </is>
       </c>
     </row>
@@ -582,29 +599,32 @@
           <t>XGBoost</t>
         </is>
       </c>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>0.0934</t>
-        </is>
+      <c r="B7" s="3" t="n">
+        <v>5000</v>
       </c>
       <c r="C7" s="3" t="inlineStr">
         <is>
-          <t>0.7558</t>
+          <t>0.0851</t>
         </is>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>
-          <t>-3.2772</t>
+          <t>0.7715</t>
         </is>
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>2.9711</t>
+          <t>-2.3997</t>
         </is>
       </c>
       <c r="F7" s="3" t="inlineStr">
         <is>
-          <t>0.0933</t>
+          <t>3.4618</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>0.0851</t>
         </is>
       </c>
     </row>
@@ -618,14 +638,14 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>(a) Elaboración propia en base a datos procesados (cluster con nscore y predicciones de modelos KNN y XGBoost). (b) n = tamaño de muestra. Desv. Est. = desviación estándar. Mín = mínimo valor observado. Máx. = máximo valor observado. Diferencia de medias = diferencia respecto a la media de datos originales.</t>
+          <t>(a) Elaboración propia en base a datos procesados (cluster con nscore y predicciones de modelos KNN y XGBoost). (b) N = número de datos. Desv. Est. = desviación estándar. Mín = mínimo valor observado. Máx. = máximo valor observado. Diferencia de medias = diferencia respecto a la media de datos originales.</t>
         </is>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:G10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>